<commit_message>
fixed the llm tuning
</commit_message>
<xml_diff>
--- a/backend/kpi/dataanalytics/medical_terms.xlsx
+++ b/backend/kpi/dataanalytics/medical_terms.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -424,13 +424,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Hypertension</v>
+        <v>pneumonoultramicroscopicsilicovolcanoconiosis</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C2">
-        <v>3.5</v>
+        <v>0.5</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -439,38 +439,38 @@
         <v>0</v>
       </c>
       <c r="F2" t="str">
-        <v>2025-10-23T05:52:19.052Z</v>
+        <v>2025-10-23T07:41:30.284Z</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Vital signs</v>
+        <v>Hypertension</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C3">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3" t="str">
-        <v>2025-10-23T05:52:19.052Z</v>
+        <v>2025-10-23T07:46:08.649Z</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>BP</v>
+        <v>Vital signs</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C4">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -479,18 +479,18 @@
         <v>0</v>
       </c>
       <c r="F4" t="str">
-        <v>2025-10-23T05:52:19.052Z</v>
+        <v>2025-10-23T07:46:08.649Z</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>HR</v>
+        <v>BP</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C5">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -499,18 +499,18 @@
         <v>0</v>
       </c>
       <c r="F5" t="str">
-        <v>2025-10-23T05:52:19.052Z</v>
+        <v>2025-10-23T07:46:08.649Z</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Temp</v>
+        <v>HR</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C6">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -519,18 +519,18 @@
         <v>0</v>
       </c>
       <c r="F6" t="str">
-        <v>2025-10-23T05:52:19.052Z</v>
+        <v>2025-10-23T07:46:08.649Z</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Diagnosis</v>
+        <v>Temp</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C7">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -539,18 +539,18 @@
         <v>0</v>
       </c>
       <c r="F7" t="str">
-        <v>2025-10-23T05:52:19.052Z</v>
+        <v>2025-10-23T07:46:08.649Z</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>Plan</v>
+        <v>Diagnosis</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C8">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -559,38 +559,38 @@
         <v>0</v>
       </c>
       <c r="F8" t="str">
-        <v>2025-10-23T05:52:19.052Z</v>
+        <v>2025-10-23T07:46:08.649Z</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>mg</v>
+        <v>Plan</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C9">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" t="str">
-        <v>2025-10-23T05:52:19.052Z</v>
+        <v>2025-10-23T07:46:08.649Z</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>daily</v>
+        <v>mg</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C10">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -599,58 +599,58 @@
         <v>1</v>
       </c>
       <c r="F10" t="str">
-        <v>2025-10-23T05:52:19.052Z</v>
+        <v>2025-10-23T07:46:08.649Z</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>Follow-up</v>
+        <v>daily</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C11">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" t="str">
-        <v>2025-10-23T05:52:19.052Z</v>
+        <v>2025-10-23T07:46:08.649Z</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>atrial fibrillation</v>
+        <v>Follow-up</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C12">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="F12" t="str">
-        <v>2025-10-23T05:52:19.052Z</v>
+        <v>2025-10-23T07:46:08.649Z</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>blood pressure</v>
+        <v>atrial fibrillation</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C13">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -659,38 +659,38 @@
         <v>0</v>
       </c>
       <c r="F13" t="str">
-        <v>2025-10-23T05:52:19.052Z</v>
+        <v>2025-10-23T07:46:08.649Z</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>Temp 36</v>
+        <v>blood pressure</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C14">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="F14" t="str">
-        <v>2025-10-23T05:52:19.052Z</v>
+        <v>2025-10-23T07:46:08.649Z</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>Aspirin 81</v>
+        <v>Temp 36</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C15">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -699,78 +699,78 @@
         <v>0</v>
       </c>
       <c r="F15" t="str">
-        <v>2025-10-23T05:52:19.052Z</v>
+        <v>2025-10-23T07:46:08.649Z</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>Palpitations</v>
+        <v>Aspirin 81</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C16">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
       <c r="F16" t="str">
-        <v>2025-10-23T05:52:19.052Z</v>
+        <v>2025-10-23T07:46:08.649Z</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>heartbeats</v>
+        <v>Palpitations</v>
       </c>
       <c r="B17">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C17">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17">
         <v>0</v>
       </c>
       <c r="F17" t="str">
-        <v>2025-10-23T05:52:19.052Z</v>
+        <v>2025-10-23T07:46:08.649Z</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>Examination</v>
+        <v>heartbeats</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C18">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
       <c r="F18" t="str">
-        <v>2025-10-23T05:52:19.052Z</v>
+        <v>2025-10-23T07:46:08.649Z</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>Extremities</v>
+        <v>Examination</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C19">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -779,58 +779,58 @@
         <v>0</v>
       </c>
       <c r="F19" t="str">
-        <v>2025-10-23T05:52:19.052Z</v>
+        <v>2025-10-23T07:46:08.649Z</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>Assessment</v>
+        <v>Extremities</v>
       </c>
       <c r="B20">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C20">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20">
         <v>0</v>
       </c>
       <c r="F20" t="str">
-        <v>2025-10-23T05:52:19.052Z</v>
+        <v>2025-10-23T07:46:08.649Z</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>fibrillation</v>
+        <v>Assessment</v>
       </c>
       <c r="B21">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C21">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21">
         <v>0</v>
       </c>
       <c r="F21" t="str">
-        <v>2025-10-23T05:52:19.052Z</v>
+        <v>2025-10-23T07:46:08.649Z</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>uncontrolled</v>
+        <v>fibrillation</v>
       </c>
       <c r="B22">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C22">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -839,38 +839,38 @@
         <v>0</v>
       </c>
       <c r="F22" t="str">
-        <v>2025-10-23T05:52:19.052Z</v>
+        <v>2025-10-23T07:46:08.649Z</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>Peripheral</v>
+        <v>uncontrolled</v>
       </c>
       <c r="B23">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C23">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23">
         <v>0</v>
       </c>
       <c r="F23" t="str">
-        <v>2025-10-23T05:52:19.052Z</v>
+        <v>2025-10-23T07:46:08.649Z</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>prevention</v>
+        <v>Peripheral</v>
       </c>
       <c r="B24">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C24">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -879,18 +879,18 @@
         <v>0</v>
       </c>
       <c r="F24" t="str">
-        <v>2025-10-23T05:52:19.052Z</v>
+        <v>2025-10-23T07:46:08.649Z</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>cardiology</v>
+        <v>prevention</v>
       </c>
       <c r="B25">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C25">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -899,18 +899,18 @@
         <v>0</v>
       </c>
       <c r="F25" t="str">
-        <v>2025-10-23T05:52:19.052Z</v>
+        <v>2025-10-23T07:46:08.649Z</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>evaluation</v>
+        <v>cardiology</v>
       </c>
       <c r="B26">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C26">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -919,32 +919,112 @@
         <v>0</v>
       </c>
       <c r="F26" t="str">
-        <v>2025-10-23T05:52:19.052Z</v>
+        <v>2025-10-23T07:46:08.649Z</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
+        <v>evaluation</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="C27">
+        <v>3.25</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" t="str">
+        <v>2025-10-23T07:46:08.649Z</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
         <v>medication</v>
       </c>
-      <c r="B27">
+      <c r="B28">
+        <v>4</v>
+      </c>
+      <c r="C28">
+        <v>3.25</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28" t="str">
+        <v>2025-10-23T07:46:08.649Z</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>infarction</v>
+      </c>
+      <c r="B29">
         <v>2</v>
       </c>
-      <c r="C27">
-        <v>3.5</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27" t="str">
-        <v>2025-10-23T05:52:19.052Z</v>
+      <c r="C29">
+        <v>3</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29" t="str">
+        <v>2025-10-23T07:47:24.691Z</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>myocardial infarction</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30" t="str">
+        <v>2025-10-23T07:47:24.693Z</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>myocardial</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <v>3</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31" t="str">
+        <v>2025-10-23T07:47:24.693Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F27"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F31"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>